<commit_message>
Add method to flag failed extractions
</commit_message>
<xml_diff>
--- a/public/publications.xlsx
+++ b/public/publications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="624">
   <si>
     <t>doi</t>
   </si>
@@ -146,6 +146,22 @@
   </si>
   <si>
     <t>2018-04-15</t>
+  </si>
+  <si>
+    <t>10.1145/3230652</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/citation.cfm?id=3230652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sikora, M., Russo, M., Đerek, J., &amp; Jurčević, A. (2018). Soundscape of an Archaeological Site Recreated with Audio Augmented Reality. ACM Transactions on Multimedia Computing, Communications, and Applications, 14(3), 1–22. doi:10.1145/3230652
+</t>
+  </si>
+  <si>
+    <t>2018-07-24</t>
+  </si>
+  <si>
+    <t>2018-07-31</t>
   </si>
   <si>
     <t>10.5334/oq.40</t>
@@ -275,6 +291,32 @@
   </si>
   <si>
     <t>2018-04-21</t>
+  </si>
+  <si>
+    <t>10.1016/j.cretres.2018.07.012</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0195667118301265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumbaa, S. L., Day, R., Gingras, M., Haggart, J. W., Holmes, R. B., Murray, A. M., &amp; Schröder-Adams, C. (2018). Lac des Bois, a locality in the Northern Western Interior Seaway (Canada) with Tethyan faunal connections during the Cenomanian/Turonian Thermal Maximum. Cretaceous Research. doi:10.1016/j.cretres.2018.07.012
+</t>
+  </si>
+  <si>
+    <t>2018-07-28</t>
+  </si>
+  <si>
+    <t>CMN 17426</t>
+  </si>
+  <si>
+    <t>10.1017/S0024282918000300</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/lichenologist/article/habitat-associations-and-distribution-model-for-fuscopannaria-leucosticta-in-nova-scotia-canada/FCE95DB86254CC7C7342548DC817A466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEARSON, K., CAMERON, R., &amp; MCMULLIN, R. T. (2018). Habitat associations and distribution model for Fuscopannaria leucosticta in Nova Scotia, Canada. The Lichenologist, 50(04), 487–497. doi:10.1017/s0024282918000300
+</t>
   </si>
   <si>
     <t>10.1017/jpa.2018.19</t>
@@ -1961,6 +2003,9 @@
   </si>
   <si>
     <t>https://digitalcommons.unl.edu/cgi/viewcontent.cgi?article=1161&amp;context=entomologypapers</t>
+  </si>
+  <si>
+    <t>CMNC CASC</t>
   </si>
   <si>
     <t>https://www.ajhtl.com/uploads/7/1/6/3/7163688/article_50_vol_7_2__2018.pdf</t>
@@ -2313,7 +2358,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J176"/>
+  <dimension ref="A1:J179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2505,21 +2550,21 @@
         <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
         <v>27</v>
@@ -2527,41 +2572,41 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" t="s">
         <v>55</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" t="s">
-        <v>57</v>
-      </c>
       <c r="H11" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>61</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>62</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>63</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2572,9 +2617,6 @@
       <c r="B13" t="s">
         <v>66</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
       <c r="D13" t="s">
         <v>67</v>
       </c>
@@ -2582,50 +2624,50 @@
         <v>68</v>
       </c>
       <c r="H13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" t="s">
         <v>72</v>
       </c>
-      <c r="B15" t="s">
+      <c r="G15" t="s">
         <v>73</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" t="s">
-        <v>75</v>
       </c>
       <c r="H15" t="s">
         <v>76</v>
+      </c>
+      <c r="I15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2635,11 +2677,11 @@
       <c r="B16" t="s">
         <v>78</v>
       </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
       <c r="D16" t="s">
         <v>79</v>
-      </c>
-      <c r="F16" t="s">
-        <v>20</v>
       </c>
       <c r="G16" t="s">
         <v>80</v>
@@ -2658,99 +2700,108 @@
       <c r="D17" t="s">
         <v>84</v>
       </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
       <c r="G17" t="s">
         <v>85</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
         <v>90</v>
       </c>
+      <c r="I18" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="H19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
         <v>96</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>97</v>
       </c>
-      <c r="D20" t="s">
+      <c r="G20" t="s">
         <v>98</v>
       </c>
-      <c r="G20" t="s">
-        <v>99</v>
-      </c>
       <c r="H20" t="s">
-        <v>100</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" t="s">
         <v>101</v>
       </c>
-      <c r="B21" t="s">
+      <c r="G21" t="s">
         <v>102</v>
       </c>
-      <c r="D21" t="s">
+      <c r="H21" t="s">
         <v>103</v>
-      </c>
-      <c r="E21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" t="s">
-        <v>104</v>
-      </c>
-      <c r="H21" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" t="s">
         <v>106</v>
       </c>
-      <c r="B22" t="s">
+      <c r="G22" t="s">
         <v>107</v>
       </c>
-      <c r="D22" t="s">
+      <c r="H22" t="s">
         <v>108</v>
-      </c>
-      <c r="G22" t="s">
-        <v>104</v>
-      </c>
-      <c r="H22" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2764,219 +2815,219 @@
         <v>111</v>
       </c>
       <c r="G23" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D24" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
       <c r="G24" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="H24" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25" t="s">
         <v>117</v>
       </c>
-      <c r="D25" t="s">
-        <v>118</v>
-      </c>
-      <c r="G25" t="s">
-        <v>104</v>
-      </c>
       <c r="H25" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="D26" t="s">
-        <v>121</v>
-      </c>
-      <c r="F26" t="s">
-        <v>20</v>
+        <v>124</v>
       </c>
       <c r="G26" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="H26" t="s">
-        <v>122</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s">
         <v>20</v>
       </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
       <c r="G27" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="H27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" t="s">
         <v>128</v>
-      </c>
-      <c r="B28" t="s">
-        <v>129</v>
-      </c>
-      <c r="D28" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" t="s">
-        <v>131</v>
-      </c>
-      <c r="H28" t="s">
-        <v>131</v>
-      </c>
-      <c r="J28" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" t="s">
         <v>133</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
         <v>134</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" t="s">
         <v>135</v>
-      </c>
-      <c r="F29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" t="s">
-        <v>136</v>
-      </c>
-      <c r="H29" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
         <v>137</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>138</v>
       </c>
-      <c r="C30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s">
         <v>139</v>
       </c>
-      <c r="E30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>140</v>
-      </c>
-      <c r="H30" t="s">
-        <v>131</v>
-      </c>
-      <c r="J30" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" t="s">
         <v>142</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>143</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" t="s">
         <v>144</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
+        <v>144</v>
+      </c>
+      <c r="J31" t="s">
         <v>145</v>
-      </c>
-      <c r="H31" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" t="s">
         <v>147</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>148</v>
       </c>
-      <c r="C32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="F32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" t="s">
         <v>149</v>
       </c>
-      <c r="G32" t="s">
-        <v>150</v>
-      </c>
       <c r="H32" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
         <v>152</v>
       </c>
-      <c r="B33" t="s">
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" t="s">
         <v>153</v>
       </c>
-      <c r="D33" t="s">
+      <c r="H33" t="s">
+        <v>144</v>
+      </c>
+      <c r="J33" t="s">
         <v>154</v>
-      </c>
-      <c r="G33" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2990,78 +3041,81 @@
         <v>157</v>
       </c>
       <c r="G34" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="H34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B35" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G35" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="H35" t="s">
-        <v>57</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B36" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" t="s">
+        <v>167</v>
+      </c>
+      <c r="G36" t="s">
         <v>163</v>
       </c>
-      <c r="D36" t="s">
-        <v>164</v>
-      </c>
-      <c r="G36" t="s">
-        <v>165</v>
-      </c>
       <c r="H36" t="s">
-        <v>146</v>
-      </c>
-      <c r="I36" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+      <c r="B37" t="s">
+        <v>169</v>
       </c>
       <c r="D37" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G37" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H37" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D38" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G38" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H38" t="s">
-        <v>174</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -3078,61 +3132,58 @@
         <v>178</v>
       </c>
       <c r="H39" t="s">
-        <v>151</v>
+        <v>159</v>
+      </c>
+      <c r="I39" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>179</v>
-      </c>
-      <c r="B40" t="s">
         <v>180</v>
       </c>
       <c r="D40" t="s">
         <v>181</v>
       </c>
-      <c r="E40" t="s">
-        <v>20</v>
-      </c>
       <c r="G40" t="s">
         <v>182</v>
       </c>
       <c r="H40" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" t="s">
         <v>184</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>185</v>
       </c>
-      <c r="D41" t="s">
+      <c r="G41" t="s">
         <v>186</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>187</v>
-      </c>
-      <c r="H41" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" t="s">
         <v>189</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
         <v>190</v>
       </c>
-      <c r="D42" t="s">
+      <c r="G42" t="s">
         <v>191</v>
       </c>
-      <c r="G42" t="s">
-        <v>187</v>
-      </c>
       <c r="H42" t="s">
-        <v>41</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -3142,22 +3193,16 @@
       <c r="B43" t="s">
         <v>193</v>
       </c>
-      <c r="C43" t="s">
-        <v>18</v>
-      </c>
       <c r="D43" t="s">
         <v>194</v>
       </c>
-      <c r="F43" t="s">
+      <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="G43" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="H43" t="s">
-        <v>195</v>
-      </c>
-      <c r="J43" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3165,424 +3210,427 @@
       <c r="A44" t="s">
         <v>197</v>
       </c>
+      <c r="B44" t="s">
+        <v>198</v>
+      </c>
       <c r="D44" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G44" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="H44" t="s">
-        <v>151</v>
+        <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B45" t="s">
+        <v>203</v>
+      </c>
+      <c r="D45" t="s">
+        <v>204</v>
+      </c>
+      <c r="G45" t="s">
         <v>200</v>
       </c>
-      <c r="D45" t="s">
-        <v>201</v>
-      </c>
-      <c r="G45" t="s">
-        <v>202</v>
-      </c>
       <c r="H45" t="s">
-        <v>203</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B46" t="s">
-        <v>205</v>
+        <v>206</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="F46" t="s">
+        <v>20</v>
       </c>
       <c r="G46" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H46" t="s">
-        <v>203</v>
+        <v>208</v>
+      </c>
+      <c r="J46" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>208</v>
-      </c>
-      <c r="B47" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D47" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G47" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H47" t="s">
-        <v>212</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48" t="s">
         <v>213</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>214</v>
       </c>
-      <c r="C48" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="G48" t="s">
         <v>215</v>
       </c>
-      <c r="F48" t="s">
-        <v>20</v>
-      </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>216</v>
-      </c>
-      <c r="H48" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
+        <v>217</v>
+      </c>
+      <c r="B49" t="s">
         <v>218</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D49" t="s">
         <v>219</v>
       </c>
-      <c r="D49" t="s">
+      <c r="G49" t="s">
         <v>220</v>
       </c>
-      <c r="G49" t="s">
-        <v>221</v>
-      </c>
       <c r="H49" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
+        <v>221</v>
+      </c>
+      <c r="B50" t="s">
+        <v>222</v>
+      </c>
+      <c r="D50" t="s">
         <v>223</v>
       </c>
-      <c r="C50" t="s">
+      <c r="G50" t="s">
         <v>224</v>
       </c>
-      <c r="D50" t="s">
+      <c r="H50" t="s">
         <v>225</v>
-      </c>
-      <c r="G50" t="s">
-        <v>221</v>
-      </c>
-      <c r="H50" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>226</v>
       </c>
+      <c r="B51" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
       <c r="D51" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+      <c r="F51" t="s">
+        <v>20</v>
       </c>
       <c r="G51" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H51" t="s">
-        <v>151</v>
-      </c>
-      <c r="J51" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="B52" t="s">
+        <v>232</v>
       </c>
       <c r="D52" t="s">
-        <v>231</v>
-      </c>
-      <c r="E52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" t="s">
-        <v>20</v>
+        <v>233</v>
       </c>
       <c r="G52" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H52" t="s">
-        <v>136</v>
-      </c>
-      <c r="I52" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
+        <v>236</v>
+      </c>
+      <c r="C53" t="s">
+        <v>237</v>
+      </c>
+      <c r="D53" t="s">
+        <v>238</v>
+      </c>
+      <c r="G53" t="s">
         <v>234</v>
       </c>
-      <c r="B53" t="s">
-        <v>235</v>
-      </c>
-      <c r="D53" t="s">
-        <v>236</v>
-      </c>
-      <c r="G53" t="s">
-        <v>237</v>
-      </c>
       <c r="H53" t="s">
-        <v>238</v>
-      </c>
-      <c r="I53" t="s">
-        <v>239</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
+        <v>239</v>
+      </c>
+      <c r="D54" t="s">
         <v>240</v>
       </c>
-      <c r="C54" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="G54" t="s">
         <v>241</v>
       </c>
-      <c r="F54" t="s">
-        <v>20</v>
-      </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
+        <v>164</v>
+      </c>
+      <c r="J54" t="s">
         <v>242</v>
-      </c>
-      <c r="H54" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>243</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
         <v>244</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" t="s">
         <v>245</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
+        <v>149</v>
+      </c>
+      <c r="I55" t="s">
         <v>246</v>
-      </c>
-      <c r="H55" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
+        <v>247</v>
+      </c>
+      <c r="B56" t="s">
         <v>248</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>249</v>
       </c>
-      <c r="D56" t="s">
+      <c r="G56" t="s">
         <v>250</v>
-      </c>
-      <c r="G56" t="s">
-        <v>246</v>
       </c>
       <c r="H56" t="s">
         <v>251</v>
       </c>
+      <c r="I56" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>252</v>
-      </c>
-      <c r="B57" t="s">
         <v>253</v>
+      </c>
+      <c r="C57" t="s">
+        <v>18</v>
       </c>
       <c r="D57" t="s">
         <v>254</v>
       </c>
+      <c r="F57" t="s">
+        <v>20</v>
+      </c>
       <c r="G57" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="H57" t="s">
-        <v>222</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B58" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D58" t="s">
-        <v>257</v>
-      </c>
-      <c r="E58" t="s">
-        <v>20</v>
+        <v>258</v>
       </c>
       <c r="G58" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="H58" t="s">
-        <v>212</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B59" t="s">
+        <v>262</v>
+      </c>
+      <c r="D59" t="s">
+        <v>263</v>
+      </c>
+      <c r="G59" t="s">
         <v>259</v>
       </c>
-      <c r="D59" t="s">
-        <v>260</v>
-      </c>
-      <c r="G59" t="s">
-        <v>246</v>
-      </c>
       <c r="H59" t="s">
-        <v>212</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B60" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D60" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="G60" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="H60" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B61" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D61" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
-      <c r="F61" t="s">
-        <v>20</v>
-      </c>
       <c r="G61" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="H61" t="s">
-        <v>188</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>267</v>
+        <v>271</v>
+      </c>
+      <c r="B62" t="s">
+        <v>272</v>
       </c>
       <c r="D62" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="G62" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="H62" t="s">
-        <v>136</v>
-      </c>
-      <c r="I62" t="s">
-        <v>269</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B63" t="s">
-        <v>271</v>
-      </c>
-      <c r="C63" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D63" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G63" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="H63" t="s">
-        <v>275</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B64" t="s">
-        <v>277</v>
-      </c>
-      <c r="C64" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D64" t="s">
-        <v>278</v>
+        <v>279</v>
+      </c>
+      <c r="E64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" t="s">
+        <v>20</v>
       </c>
       <c r="G64" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="H64" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>279</v>
-      </c>
-      <c r="B65" t="s">
         <v>280</v>
       </c>
       <c r="D65" t="s">
         <v>281</v>
       </c>
       <c r="G65" t="s">
+        <v>259</v>
+      </c>
+      <c r="H65" t="s">
+        <v>149</v>
+      </c>
+      <c r="I65" t="s">
         <v>282</v>
-      </c>
-      <c r="H65" t="s">
-        <v>283</v>
-      </c>
-      <c r="J65" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
+        <v>283</v>
+      </c>
+      <c r="B66" t="s">
+        <v>284</v>
+      </c>
+      <c r="C66" t="s">
         <v>285</v>
       </c>
-      <c r="B66" t="s">
+      <c r="D66" t="s">
         <v>286</v>
       </c>
-      <c r="D66" t="s">
+      <c r="G66" t="s">
         <v>287</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>288</v>
-      </c>
-      <c r="H66" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -3592,54 +3640,54 @@
       <c r="B67" t="s">
         <v>290</v>
       </c>
+      <c r="C67" t="s">
+        <v>285</v>
+      </c>
       <c r="D67" t="s">
         <v>291</v>
       </c>
       <c r="G67" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H67" t="s">
-        <v>293</v>
-      </c>
-      <c r="I67" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
+        <v>292</v>
+      </c>
+      <c r="B68" t="s">
+        <v>293</v>
+      </c>
+      <c r="D68" t="s">
+        <v>294</v>
+      </c>
+      <c r="G68" t="s">
         <v>295</v>
       </c>
-      <c r="B68" t="s">
+      <c r="H68" t="s">
         <v>296</v>
       </c>
-      <c r="D68" t="s">
+      <c r="J68" t="s">
         <v>297</v>
-      </c>
-      <c r="G68" t="s">
-        <v>298</v>
-      </c>
-      <c r="H68" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
+        <v>298</v>
+      </c>
+      <c r="B69" t="s">
         <v>299</v>
-      </c>
-      <c r="C69" t="s">
-        <v>18</v>
       </c>
       <c r="D69" t="s">
         <v>300</v>
       </c>
       <c r="G69" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="H69" t="s">
-        <v>242</v>
-      </c>
-      <c r="I69" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -3652,339 +3700,336 @@
       <c r="D70" t="s">
         <v>304</v>
       </c>
-      <c r="E70" t="s">
-        <v>20</v>
-      </c>
       <c r="G70" t="s">
         <v>305</v>
       </c>
       <c r="H70" t="s">
-        <v>292</v>
+        <v>306</v>
+      </c>
+      <c r="I70" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
+        <v>308</v>
+      </c>
+      <c r="B71" t="s">
+        <v>309</v>
+      </c>
+      <c r="D71" t="s">
+        <v>310</v>
+      </c>
+      <c r="G71" t="s">
+        <v>311</v>
+      </c>
+      <c r="H71" t="s">
         <v>306</v>
-      </c>
-      <c r="B71" t="s">
-        <v>307</v>
-      </c>
-      <c r="C71" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71" t="s">
-        <v>308</v>
-      </c>
-      <c r="E71" t="s">
-        <v>20</v>
-      </c>
-      <c r="G71" t="s">
-        <v>309</v>
-      </c>
-      <c r="H71" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>311</v>
-      </c>
-      <c r="B72" t="s">
         <v>312</v>
+      </c>
+      <c r="C72" t="s">
+        <v>18</v>
       </c>
       <c r="D72" t="s">
         <v>313</v>
       </c>
       <c r="G72" t="s">
+        <v>311</v>
+      </c>
+      <c r="H72" t="s">
+        <v>255</v>
+      </c>
+      <c r="I72" t="s">
         <v>314</v>
-      </c>
-      <c r="H72" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
+        <v>315</v>
+      </c>
+      <c r="B73" t="s">
         <v>316</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>317</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" t="s">
         <v>318</v>
       </c>
-      <c r="G73" t="s">
-        <v>319</v>
-      </c>
       <c r="H73" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
+        <v>319</v>
+      </c>
+      <c r="B74" t="s">
+        <v>320</v>
+      </c>
+      <c r="C74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" t="s">
         <v>321</v>
       </c>
-      <c r="B74" t="s">
+      <c r="E74" t="s">
+        <v>20</v>
+      </c>
+      <c r="G74" t="s">
         <v>322</v>
       </c>
-      <c r="D74" t="s">
+      <c r="H74" t="s">
         <v>323</v>
-      </c>
-      <c r="G74" t="s">
-        <v>319</v>
-      </c>
-      <c r="H74" t="s">
-        <v>292</v>
-      </c>
-      <c r="I74" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
+        <v>324</v>
+      </c>
+      <c r="B75" t="s">
         <v>325</v>
       </c>
-      <c r="B75" t="s">
+      <c r="D75" t="s">
         <v>326</v>
       </c>
-      <c r="D75" t="s">
+      <c r="G75" t="s">
         <v>327</v>
       </c>
-      <c r="G75" t="s">
-        <v>319</v>
-      </c>
       <c r="H75" t="s">
-        <v>293</v>
+        <v>328</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B76" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D76" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G76" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="H76" t="s">
-        <v>282</v>
-      </c>
-      <c r="I76" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
+        <v>334</v>
+      </c>
+      <c r="B77" t="s">
+        <v>335</v>
+      </c>
+      <c r="D77" t="s">
+        <v>336</v>
+      </c>
+      <c r="G77" t="s">
         <v>332</v>
       </c>
-      <c r="B77" t="s">
-        <v>333</v>
-      </c>
-      <c r="C77" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77" t="s">
-        <v>334</v>
-      </c>
-      <c r="E77" t="s">
-        <v>20</v>
-      </c>
-      <c r="G77" t="s">
-        <v>319</v>
-      </c>
       <c r="H77" t="s">
-        <v>221</v>
+        <v>305</v>
+      </c>
+      <c r="I77" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B78" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D78" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="G78" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="H78" t="s">
-        <v>183</v>
+        <v>306</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>338</v>
+        <v>341</v>
+      </c>
+      <c r="B79" t="s">
+        <v>342</v>
       </c>
       <c r="D79" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="G79" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="H79" t="s">
-        <v>136</v>
+        <v>295</v>
+      </c>
+      <c r="I79" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="B80" t="s">
-        <v>341</v>
+        <v>346</v>
+      </c>
+      <c r="C80" t="s">
+        <v>18</v>
       </c>
       <c r="D80" t="s">
-        <v>342</v>
+        <v>347</v>
+      </c>
+      <c r="E80" t="s">
+        <v>20</v>
       </c>
       <c r="G80" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="H80" t="s">
-        <v>275</v>
+        <v>234</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>344</v>
+        <v>348</v>
+      </c>
+      <c r="B81" t="s">
+        <v>349</v>
       </c>
       <c r="D81" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="G81" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="H81" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>346</v>
-      </c>
-      <c r="B82" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="D82" t="s">
-        <v>348</v>
-      </c>
-      <c r="E82" t="s">
-        <v>20</v>
+        <v>352</v>
       </c>
       <c r="G82" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="H82" t="s">
-        <v>275</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B83" t="s">
-        <v>351</v>
-      </c>
-      <c r="C83" t="s">
-        <v>18</v>
+        <v>354</v>
       </c>
       <c r="D83" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="G83" t="s">
-        <v>14</v>
+        <v>356</v>
       </c>
       <c r="H83" t="s">
-        <v>353</v>
-      </c>
-      <c r="I83" t="s">
-        <v>354</v>
+        <v>288</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>355</v>
-      </c>
-      <c r="B84" t="s">
+        <v>357</v>
+      </c>
+      <c r="D84" t="s">
+        <v>358</v>
+      </c>
+      <c r="G84" t="s">
         <v>356</v>
       </c>
-      <c r="C84" t="s">
-        <v>18</v>
-      </c>
-      <c r="D84" t="s">
-        <v>357</v>
-      </c>
-      <c r="G84" t="s">
-        <v>358</v>
-      </c>
       <c r="H84" t="s">
-        <v>14</v>
-      </c>
-      <c r="I84" t="s">
-        <v>359</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
+        <v>359</v>
+      </c>
+      <c r="B85" t="s">
         <v>360</v>
       </c>
-      <c r="B85" t="s">
+      <c r="D85" t="s">
         <v>361</v>
       </c>
-      <c r="C85" t="s">
-        <v>18</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+      <c r="G85" t="s">
         <v>362</v>
       </c>
-      <c r="E85" t="s">
-        <v>20</v>
-      </c>
-      <c r="G85" t="s">
-        <v>363</v>
-      </c>
       <c r="H85" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
+        <v>363</v>
+      </c>
+      <c r="B86" t="s">
         <v>364</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86" t="s">
         <v>365</v>
       </c>
-      <c r="D86" t="s">
+      <c r="G86" t="s">
+        <v>14</v>
+      </c>
+      <c r="H86" t="s">
         <v>366</v>
       </c>
-      <c r="G86" t="s">
+      <c r="I86" t="s">
         <v>367</v>
-      </c>
-      <c r="H86" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
+        <v>368</v>
+      </c>
+      <c r="B87" t="s">
         <v>369</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" t="s">
         <v>370</v>
       </c>
-      <c r="D87" t="s">
+      <c r="G87" t="s">
         <v>371</v>
       </c>
-      <c r="F87" t="s">
-        <v>20</v>
-      </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" t="s">
         <v>372</v>
-      </c>
-      <c r="H87" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3994,14 +4039,20 @@
       <c r="B88" t="s">
         <v>374</v>
       </c>
+      <c r="C88" t="s">
+        <v>18</v>
+      </c>
       <c r="D88" t="s">
         <v>375</v>
       </c>
+      <c r="E88" t="s">
+        <v>20</v>
+      </c>
       <c r="G88" t="s">
         <v>376</v>
       </c>
       <c r="H88" t="s">
-        <v>349</v>
+        <v>288</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -4015,289 +4066,286 @@
         <v>379</v>
       </c>
       <c r="G89" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="H89" t="s">
-        <v>222</v>
+        <v>381</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B90" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D90" t="s">
-        <v>382</v>
+        <v>384</v>
+      </c>
+      <c r="F90" t="s">
+        <v>20</v>
       </c>
       <c r="G90" t="s">
+        <v>385</v>
+      </c>
+      <c r="H90" t="s">
         <v>376</v>
-      </c>
-      <c r="H90" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B91" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="D91" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="G91" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="H91" t="s">
-        <v>195</v>
+        <v>362</v>
       </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B92" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="D92" t="s">
-        <v>388</v>
-      </c>
-      <c r="F92" t="s">
-        <v>20</v>
-      </c>
-      <c r="G92">
-        <v>2018</v>
+        <v>392</v>
+      </c>
+      <c r="G92" t="s">
+        <v>389</v>
       </c>
       <c r="H92" t="s">
-        <v>389</v>
+        <v>235</v>
       </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B93" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="D93" t="s">
-        <v>392</v>
-      </c>
-      <c r="G93">
-        <v>2018</v>
+        <v>395</v>
+      </c>
+      <c r="G93" t="s">
+        <v>389</v>
       </c>
       <c r="H93" t="s">
-        <v>389</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B94" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="D94" t="s">
-        <v>395</v>
-      </c>
-      <c r="G94">
-        <v>2018</v>
+        <v>398</v>
+      </c>
+      <c r="G94" t="s">
+        <v>389</v>
       </c>
       <c r="H94" t="s">
-        <v>389</v>
+        <v>208</v>
       </c>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B95" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="D95" t="s">
-        <v>398</v>
+        <v>401</v>
+      </c>
+      <c r="F95" t="s">
+        <v>20</v>
       </c>
       <c r="G95">
         <v>2018</v>
       </c>
       <c r="H95" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="B96" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="D96" t="s">
-        <v>402</v>
-      </c>
-      <c r="F96" t="s">
-        <v>20</v>
+        <v>405</v>
       </c>
       <c r="G96">
         <v>2018</v>
       </c>
       <c r="H96" t="s">
-        <v>275</v>
+        <v>402</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B97" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="D97" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="G97">
         <v>2018</v>
       </c>
       <c r="H97" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B98" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D98" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="G98">
         <v>2018</v>
       </c>
       <c r="H98" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B99" t="s">
-        <v>411</v>
-      </c>
-      <c r="C99" t="s">
-        <v>272</v>
+        <v>414</v>
       </c>
       <c r="D99" t="s">
-        <v>412</v>
+        <v>415</v>
+      </c>
+      <c r="F99" t="s">
+        <v>20</v>
       </c>
       <c r="G99">
         <v>2018</v>
       </c>
       <c r="H99" t="s">
-        <v>81</v>
+        <v>288</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B100" t="s">
-        <v>414</v>
-      </c>
-      <c r="C100" t="s">
-        <v>18</v>
+        <v>417</v>
       </c>
       <c r="D100" t="s">
-        <v>415</v>
-      </c>
-      <c r="G100" t="s">
-        <v>416</v>
+        <v>418</v>
+      </c>
+      <c r="G100">
+        <v>2018</v>
       </c>
       <c r="H100" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B101" t="s">
+        <v>421</v>
+      </c>
+      <c r="D101" t="s">
+        <v>422</v>
+      </c>
+      <c r="G101">
+        <v>2018</v>
+      </c>
+      <c r="H101" t="s">
         <v>419</v>
-      </c>
-      <c r="C101" t="s">
-        <v>420</v>
-      </c>
-      <c r="D101" t="s">
-        <v>421</v>
-      </c>
-      <c r="G101" t="s">
-        <v>422</v>
-      </c>
-      <c r="H101" t="s">
-        <v>423</v>
-      </c>
-      <c r="I101" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" t="s">
+        <v>423</v>
+      </c>
+      <c r="B102" t="s">
+        <v>424</v>
+      </c>
+      <c r="C102" t="s">
+        <v>285</v>
+      </c>
+      <c r="D102" t="s">
         <v>425</v>
       </c>
-      <c r="B102" t="s">
-        <v>426</v>
-      </c>
-      <c r="D102" t="s">
-        <v>427</v>
-      </c>
-      <c r="G102" t="s">
-        <v>428</v>
+      <c r="G102">
+        <v>2018</v>
       </c>
       <c r="H102" t="s">
-        <v>429</v>
+        <v>86</v>
       </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" t="s">
+        <v>426</v>
+      </c>
+      <c r="B103" t="s">
+        <v>427</v>
+      </c>
+      <c r="C103" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103" t="s">
+        <v>428</v>
+      </c>
+      <c r="G103" t="s">
+        <v>429</v>
+      </c>
+      <c r="H103" t="s">
         <v>430</v>
-      </c>
-      <c r="B103" t="s">
-        <v>431</v>
-      </c>
-      <c r="D103" t="s">
-        <v>432</v>
-      </c>
-      <c r="E103" t="s">
-        <v>20</v>
-      </c>
-      <c r="G103" t="s">
-        <v>433</v>
-      </c>
-      <c r="H103" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" t="s">
+        <v>431</v>
+      </c>
+      <c r="B104" t="s">
+        <v>432</v>
+      </c>
+      <c r="C104" t="s">
+        <v>433</v>
+      </c>
+      <c r="D104" t="s">
         <v>434</v>
       </c>
-      <c r="B104" t="s">
+      <c r="G104" t="s">
         <v>435</v>
       </c>
-      <c r="C104" t="s">
-        <v>18</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="H104" t="s">
         <v>436</v>
       </c>
-      <c r="G104" t="s">
+      <c r="I104" t="s">
         <v>437</v>
-      </c>
-      <c r="H104" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -4334,66 +4382,66 @@
         <v>446</v>
       </c>
       <c r="H106" t="s">
-        <v>447</v>
-      </c>
-      <c r="J106" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" t="s">
+        <v>447</v>
+      </c>
+      <c r="B107" t="s">
+        <v>448</v>
+      </c>
+      <c r="C107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D107" t="s">
         <v>449</v>
       </c>
-      <c r="B107" t="s">
+      <c r="G107" t="s">
         <v>450</v>
       </c>
-      <c r="D107" t="s">
-        <v>451</v>
-      </c>
-      <c r="G107" t="s">
-        <v>446</v>
-      </c>
       <c r="H107" t="s">
-        <v>442</v>
-      </c>
-      <c r="I107" t="s">
-        <v>452</v>
+        <v>164</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" t="s">
+        <v>451</v>
+      </c>
+      <c r="B108" t="s">
+        <v>452</v>
+      </c>
+      <c r="D108" t="s">
         <v>453</v>
       </c>
-      <c r="B108" t="s">
+      <c r="G108" t="s">
         <v>454</v>
       </c>
-      <c r="C108" t="s">
+      <c r="H108" t="s">
         <v>455</v>
-      </c>
-      <c r="D108" t="s">
-        <v>456</v>
-      </c>
-      <c r="G108" t="s">
-        <v>446</v>
-      </c>
-      <c r="H108" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" t="s">
+        <v>456</v>
+      </c>
+      <c r="B109" t="s">
+        <v>457</v>
+      </c>
+      <c r="D109" t="s">
         <v>458</v>
       </c>
-      <c r="B109" t="s">
+      <c r="E109" t="s">
+        <v>20</v>
+      </c>
+      <c r="G109" t="s">
         <v>459</v>
       </c>
-      <c r="D109" t="s">
+      <c r="H109" t="s">
         <v>460</v>
       </c>
-      <c r="G109" t="s">
-        <v>446</v>
-      </c>
-      <c r="H109" t="s">
+      <c r="J109" t="s">
         <v>461</v>
       </c>
     </row>
@@ -4404,185 +4452,185 @@
       <c r="B110" t="s">
         <v>463</v>
       </c>
-      <c r="C110" t="s">
-        <v>18</v>
-      </c>
       <c r="D110" t="s">
         <v>464</v>
       </c>
-      <c r="E110" t="s">
-        <v>20</v>
-      </c>
-      <c r="F110" t="s">
-        <v>20</v>
-      </c>
       <c r="G110" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="H110" t="s">
+        <v>455</v>
+      </c>
+      <c r="I110" t="s">
         <v>465</v>
-      </c>
-      <c r="I110" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" t="s">
+        <v>466</v>
+      </c>
+      <c r="B111" t="s">
         <v>467</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>468</v>
-      </c>
-      <c r="C111" t="s">
-        <v>18</v>
       </c>
       <c r="D111" t="s">
         <v>469</v>
       </c>
-      <c r="F111" t="s">
-        <v>20</v>
-      </c>
       <c r="G111" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="H111" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B112" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D112" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G112" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="H112" t="s">
-        <v>417</v>
-      </c>
-      <c r="I112" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B113" t="s">
-        <v>475</v>
+        <v>476</v>
+      </c>
+      <c r="C113" t="s">
+        <v>18</v>
       </c>
       <c r="D113" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E113" t="s">
         <v>20</v>
       </c>
+      <c r="F113" t="s">
+        <v>20</v>
+      </c>
       <c r="G113" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="H113" t="s">
-        <v>363</v>
+        <v>478</v>
+      </c>
+      <c r="I113" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B114" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C114" t="s">
         <v>18</v>
       </c>
       <c r="D114" t="s">
-        <v>479</v>
+        <v>482</v>
+      </c>
+      <c r="F114" t="s">
+        <v>20</v>
       </c>
       <c r="G114" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="H114" t="s">
-        <v>151</v>
+        <v>474</v>
       </c>
     </row>
     <row r="115" spans="1:10">
       <c r="A115" t="s">
-        <v>480</v>
+        <v>483</v>
+      </c>
+      <c r="B115" t="s">
+        <v>484</v>
       </c>
       <c r="D115" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="G115" t="s">
-        <v>446</v>
+        <v>459</v>
       </c>
       <c r="H115" t="s">
-        <v>151</v>
+        <v>430</v>
+      </c>
+      <c r="I115" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="116" spans="1:10">
       <c r="A116" t="s">
-        <v>267</v>
+        <v>487</v>
       </c>
       <c r="B116" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="D116" t="s">
-        <v>483</v>
+        <v>489</v>
+      </c>
+      <c r="E116" t="s">
+        <v>20</v>
       </c>
       <c r="G116" t="s">
-        <v>389</v>
+        <v>459</v>
       </c>
       <c r="H116" t="s">
-        <v>429</v>
-      </c>
-      <c r="I116" t="s">
-        <v>269</v>
+        <v>376</v>
       </c>
     </row>
     <row r="117" spans="1:10">
       <c r="A117" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="B117" t="s">
-        <v>485</v>
+        <v>491</v>
+      </c>
+      <c r="C117" t="s">
+        <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="G117" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
       <c r="H117" t="s">
-        <v>447</v>
-      </c>
-      <c r="I117" t="s">
-        <v>488</v>
+        <v>164</v>
       </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118" t="s">
-        <v>489</v>
-      </c>
-      <c r="B118" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="D118" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="G118" t="s">
-        <v>492</v>
+        <v>459</v>
       </c>
       <c r="H118" t="s">
-        <v>493</v>
+        <v>164</v>
       </c>
     </row>
     <row r="119" spans="1:10">
       <c r="A119" t="s">
-        <v>494</v>
+        <v>280</v>
       </c>
       <c r="B119" t="s">
         <v>495</v>
@@ -4590,31 +4638,31 @@
       <c r="D119" t="s">
         <v>496</v>
       </c>
-      <c r="F119" t="s">
-        <v>20</v>
-      </c>
       <c r="G119" t="s">
-        <v>497</v>
+        <v>402</v>
       </c>
       <c r="H119" t="s">
-        <v>447</v>
+        <v>442</v>
+      </c>
+      <c r="I119" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="120" spans="1:10">
       <c r="A120" t="s">
+        <v>497</v>
+      </c>
+      <c r="B120" t="s">
         <v>498</v>
       </c>
-      <c r="B120" t="s">
+      <c r="D120" t="s">
         <v>499</v>
       </c>
-      <c r="D120" t="s">
+      <c r="G120" t="s">
         <v>500</v>
       </c>
-      <c r="G120" t="s">
-        <v>497</v>
-      </c>
       <c r="H120" t="s">
-        <v>447</v>
+        <v>460</v>
       </c>
       <c r="I120" t="s">
         <v>501</v>
@@ -4631,654 +4679,714 @@
         <v>504</v>
       </c>
       <c r="G121" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="H121" t="s">
-        <v>447</v>
-      </c>
-      <c r="I121" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B122" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D122" t="s">
-        <v>508</v>
-      </c>
-      <c r="E122" t="s">
+        <v>509</v>
+      </c>
+      <c r="F122" t="s">
         <v>20</v>
       </c>
       <c r="G122" t="s">
-        <v>497</v>
+        <v>510</v>
       </c>
       <c r="H122" t="s">
-        <v>509</v>
+        <v>460</v>
       </c>
     </row>
     <row r="123" spans="1:10">
       <c r="A123" t="s">
+        <v>511</v>
+      </c>
+      <c r="B123" t="s">
+        <v>512</v>
+      </c>
+      <c r="D123" t="s">
+        <v>513</v>
+      </c>
+      <c r="G123" t="s">
         <v>510</v>
       </c>
-      <c r="B123" t="s">
-        <v>511</v>
-      </c>
-      <c r="D123" t="s">
-        <v>512</v>
-      </c>
-      <c r="G123" t="s">
-        <v>497</v>
-      </c>
       <c r="H123" t="s">
-        <v>429</v>
+        <v>460</v>
+      </c>
+      <c r="I123" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" t="s">
-        <v>513</v>
+        <v>515</v>
+      </c>
+      <c r="B124" t="s">
+        <v>516</v>
       </c>
       <c r="D124" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="G124" t="s">
-        <v>497</v>
+        <v>510</v>
       </c>
       <c r="H124" t="s">
-        <v>151</v>
-      </c>
-      <c r="J124" t="s">
-        <v>515</v>
+        <v>460</v>
+      </c>
+      <c r="I124" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B125" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="D125" t="s">
-        <v>518</v>
+        <v>521</v>
+      </c>
+      <c r="E125" t="s">
+        <v>20</v>
       </c>
       <c r="G125" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="H125" t="s">
-        <v>151</v>
+        <v>522</v>
       </c>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B126" t="s">
-        <v>521</v>
-      </c>
-      <c r="C126" t="s">
-        <v>18</v>
+        <v>524</v>
       </c>
       <c r="D126" t="s">
-        <v>522</v>
-      </c>
-      <c r="E126" t="s">
-        <v>20</v>
+        <v>525</v>
       </c>
       <c r="G126" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="H126" t="s">
-        <v>524</v>
-      </c>
-      <c r="I126" t="s">
-        <v>525</v>
+        <v>442</v>
       </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" t="s">
         <v>526</v>
       </c>
-      <c r="B127" t="s">
+      <c r="D127" t="s">
         <v>527</v>
       </c>
-      <c r="E127" t="s">
-        <v>20</v>
+      <c r="G127" t="s">
+        <v>510</v>
       </c>
       <c r="H127" t="s">
-        <v>368</v>
+        <v>164</v>
+      </c>
+      <c r="J127" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="128" spans="1:10">
       <c r="A128" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B128" t="s">
-        <v>529</v>
-      </c>
-      <c r="F128" t="s">
-        <v>20</v>
+        <v>530</v>
+      </c>
+      <c r="D128" t="s">
+        <v>531</v>
+      </c>
+      <c r="G128" t="s">
+        <v>532</v>
       </c>
       <c r="H128" t="s">
-        <v>282</v>
+        <v>164</v>
       </c>
     </row>
     <row r="129" spans="1:9">
       <c r="A129" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B129" t="s">
-        <v>531</v>
+        <v>534</v>
+      </c>
+      <c r="C129" t="s">
+        <v>18</v>
+      </c>
+      <c r="D129" t="s">
+        <v>535</v>
       </c>
       <c r="E129" t="s">
         <v>20</v>
       </c>
+      <c r="G129" t="s">
+        <v>536</v>
+      </c>
       <c r="H129" t="s">
-        <v>532</v>
+        <v>537</v>
+      </c>
+      <c r="I129" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="130" spans="1:9">
       <c r="A130" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="B130" t="s">
-        <v>534</v>
-      </c>
-      <c r="D130" t="s">
-        <v>535</v>
+        <v>540</v>
+      </c>
+      <c r="E130" t="s">
+        <v>20</v>
       </c>
       <c r="H130" t="s">
-        <v>447</v>
-      </c>
-      <c r="I130" t="s">
-        <v>59</v>
+        <v>381</v>
       </c>
     </row>
     <row r="131" spans="1:9">
       <c r="A131" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="B131" t="s">
-        <v>537</v>
-      </c>
-      <c r="C131" t="s">
-        <v>18</v>
-      </c>
-      <c r="D131" t="s">
-        <v>538</v>
-      </c>
-      <c r="E131" t="s">
-        <v>20</v>
+        <v>542</v>
       </c>
       <c r="F131" t="s">
         <v>20</v>
       </c>
       <c r="H131" t="s">
-        <v>217</v>
+        <v>295</v>
       </c>
     </row>
     <row r="132" spans="1:9">
       <c r="A132" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="B132" t="s">
-        <v>540</v>
-      </c>
-      <c r="C132" t="s">
-        <v>18</v>
-      </c>
-      <c r="D132" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="E132" t="s">
         <v>20</v>
       </c>
-      <c r="F132" t="s">
-        <v>20</v>
-      </c>
       <c r="H132" t="s">
-        <v>188</v>
+        <v>545</v>
       </c>
     </row>
     <row r="133" spans="1:9">
       <c r="A133" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="B133" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="D133" t="s">
-        <v>544</v>
-      </c>
-      <c r="E133" t="s">
-        <v>20</v>
-      </c>
-      <c r="F133" t="s">
-        <v>20</v>
+        <v>548</v>
       </c>
       <c r="H133" t="s">
-        <v>545</v>
+        <v>460</v>
+      </c>
+      <c r="I133" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B134" t="s">
-        <v>547</v>
+        <v>550</v>
+      </c>
+      <c r="C134" t="s">
+        <v>18</v>
+      </c>
+      <c r="D134" t="s">
+        <v>551</v>
+      </c>
+      <c r="E134" t="s">
+        <v>20</v>
+      </c>
+      <c r="F134" t="s">
+        <v>20</v>
       </c>
       <c r="H134" t="s">
-        <v>41</v>
+        <v>230</v>
       </c>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="B135" t="s">
-        <v>549</v>
+        <v>553</v>
+      </c>
+      <c r="C135" t="s">
+        <v>18</v>
+      </c>
+      <c r="D135" t="s">
+        <v>554</v>
+      </c>
+      <c r="E135" t="s">
+        <v>20</v>
+      </c>
+      <c r="F135" t="s">
+        <v>20</v>
       </c>
       <c r="H135" t="s">
-        <v>131</v>
-      </c>
-      <c r="I135" t="s">
-        <v>550</v>
+        <v>201</v>
       </c>
     </row>
     <row r="136" spans="1:9">
       <c r="A136" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="B136" t="s">
-        <v>551</v>
+        <v>556</v>
+      </c>
+      <c r="D136" t="s">
+        <v>557</v>
+      </c>
+      <c r="E136" t="s">
+        <v>20</v>
+      </c>
+      <c r="F136" t="s">
+        <v>20</v>
       </c>
       <c r="H136" t="s">
-        <v>131</v>
-      </c>
-      <c r="I136" t="s">
-        <v>550</v>
+        <v>558</v>
       </c>
     </row>
     <row r="137" spans="1:9">
       <c r="A137" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="B137" t="s">
-        <v>553</v>
-      </c>
-      <c r="C137" t="s">
-        <v>18</v>
+        <v>560</v>
       </c>
       <c r="H137" t="s">
-        <v>127</v>
-      </c>
-      <c r="I137" t="s">
-        <v>554</v>
+        <v>41</v>
       </c>
     </row>
     <row r="138" spans="1:9">
       <c r="A138" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="B138" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c r="H138" t="s">
-        <v>122</v>
+        <v>144</v>
+      </c>
+      <c r="I138" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="B139" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="H139" t="s">
-        <v>559</v>
+        <v>144</v>
+      </c>
+      <c r="I139" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="140" spans="1:9">
       <c r="A140" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="B140" t="s">
-        <v>561</v>
-      </c>
-      <c r="D140" t="s">
-        <v>562</v>
+        <v>566</v>
+      </c>
+      <c r="C140" t="s">
+        <v>18</v>
       </c>
       <c r="H140" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="I140" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="B141" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="H141" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
     </row>
     <row r="142" spans="1:9">
+      <c r="A142" t="s">
+        <v>570</v>
+      </c>
       <c r="B142" t="s">
-        <v>566</v>
-      </c>
-      <c r="F142" t="s">
-        <v>20</v>
+        <v>571</v>
       </c>
       <c r="H142" t="s">
-        <v>447</v>
+        <v>572</v>
       </c>
     </row>
     <row r="143" spans="1:9">
+      <c r="A143" t="s">
+        <v>573</v>
+      </c>
       <c r="B143" t="s">
-        <v>567</v>
+        <v>574</v>
+      </c>
+      <c r="D143" t="s">
+        <v>575</v>
       </c>
       <c r="H143" t="s">
-        <v>568</v>
+        <v>69</v>
+      </c>
+      <c r="I143" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="144" spans="1:9">
+      <c r="A144" t="s">
+        <v>577</v>
+      </c>
       <c r="B144" t="s">
-        <v>569</v>
+        <v>578</v>
       </c>
       <c r="H144" t="s">
-        <v>509</v>
+        <v>51</v>
       </c>
     </row>
     <row r="145" spans="2:9">
       <c r="B145" t="s">
-        <v>570</v>
+        <v>579</v>
+      </c>
+      <c r="F145" t="s">
+        <v>20</v>
       </c>
       <c r="H145" t="s">
-        <v>399</v>
+        <v>460</v>
       </c>
     </row>
     <row r="146" spans="2:9">
       <c r="B146" t="s">
-        <v>571</v>
+        <v>580</v>
       </c>
       <c r="H146" t="s">
-        <v>399</v>
+        <v>581</v>
       </c>
     </row>
     <row r="147" spans="2:9">
       <c r="B147" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
       <c r="H147" t="s">
-        <v>399</v>
+        <v>522</v>
       </c>
     </row>
     <row r="148" spans="2:9">
       <c r="B148" t="s">
-        <v>573</v>
+        <v>583</v>
       </c>
       <c r="H148" t="s">
-        <v>574</v>
+        <v>412</v>
       </c>
     </row>
     <row r="149" spans="2:9">
       <c r="B149" t="s">
-        <v>575</v>
+        <v>584</v>
       </c>
       <c r="H149" t="s">
-        <v>442</v>
+        <v>412</v>
       </c>
     </row>
     <row r="150" spans="2:9">
       <c r="B150" t="s">
-        <v>576</v>
+        <v>585</v>
       </c>
       <c r="H150" t="s">
-        <v>457</v>
+        <v>412</v>
       </c>
     </row>
     <row r="151" spans="2:9">
       <c r="B151" t="s">
-        <v>577</v>
-      </c>
-      <c r="E151" t="s">
-        <v>20</v>
-      </c>
-      <c r="F151" t="s">
-        <v>20</v>
+        <v>586</v>
       </c>
       <c r="H151" t="s">
-        <v>461</v>
-      </c>
-      <c r="I151" t="s">
-        <v>578</v>
+        <v>587</v>
       </c>
     </row>
     <row r="152" spans="2:9">
       <c r="B152" t="s">
-        <v>579</v>
+        <v>588</v>
       </c>
       <c r="H152" t="s">
-        <v>580</v>
+        <v>455</v>
       </c>
     </row>
     <row r="153" spans="2:9">
       <c r="B153" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="H153" t="s">
-        <v>353</v>
+        <v>470</v>
       </c>
     </row>
     <row r="154" spans="2:9">
       <c r="B154" t="s">
-        <v>582</v>
+        <v>590</v>
+      </c>
+      <c r="E154" t="s">
+        <v>20</v>
+      </c>
+      <c r="F154" t="s">
+        <v>20</v>
       </c>
       <c r="H154" t="s">
-        <v>320</v>
+        <v>474</v>
+      </c>
+      <c r="I154" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="155" spans="2:9">
       <c r="B155" t="s">
-        <v>583</v>
+        <v>592</v>
       </c>
       <c r="H155" t="s">
-        <v>320</v>
+        <v>593</v>
       </c>
     </row>
     <row r="156" spans="2:9">
       <c r="B156" t="s">
-        <v>584</v>
+        <v>594</v>
       </c>
       <c r="H156" t="s">
-        <v>292</v>
+        <v>366</v>
       </c>
     </row>
     <row r="157" spans="2:9">
       <c r="B157" t="s">
-        <v>585</v>
+        <v>595</v>
       </c>
       <c r="H157" t="s">
-        <v>293</v>
+        <v>333</v>
       </c>
     </row>
     <row r="158" spans="2:9">
       <c r="B158" t="s">
-        <v>586</v>
+        <v>596</v>
       </c>
       <c r="H158" t="s">
-        <v>21</v>
+        <v>333</v>
       </c>
     </row>
     <row r="159" spans="2:9">
       <c r="B159" t="s">
-        <v>587</v>
-      </c>
-      <c r="F159" t="s">
-        <v>20</v>
+        <v>597</v>
       </c>
       <c r="H159" t="s">
-        <v>238</v>
+        <v>305</v>
       </c>
     </row>
     <row r="160" spans="2:9">
       <c r="B160" t="s">
-        <v>588</v>
-      </c>
-      <c r="E160" t="s">
-        <v>20</v>
-      </c>
-      <c r="F160" t="s">
-        <v>20</v>
+        <v>598</v>
       </c>
       <c r="H160" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="161" spans="2:10">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="161" spans="2:9">
       <c r="B161" t="s">
-        <v>589</v>
+        <v>599</v>
       </c>
       <c r="H161" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="162" spans="2:9">
+      <c r="B162" t="s">
+        <v>600</v>
+      </c>
+      <c r="F162" t="s">
+        <v>20</v>
+      </c>
+      <c r="H162" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="162" spans="2:10">
-      <c r="B162" t="s">
-        <v>590</v>
-      </c>
-      <c r="H162" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="163" spans="2:10">
+    <row r="163" spans="2:9">
       <c r="B163" t="s">
-        <v>592</v>
+        <v>601</v>
+      </c>
+      <c r="E163" t="s">
+        <v>20</v>
       </c>
       <c r="F163" t="s">
         <v>20</v>
       </c>
       <c r="H163" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="164" spans="2:10">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="164" spans="2:9">
       <c r="B164" t="s">
-        <v>594</v>
-      </c>
-      <c r="F164" t="s">
-        <v>20</v>
+        <v>602</v>
       </c>
       <c r="H164" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="165" spans="2:10">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="165" spans="2:9">
       <c r="B165" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="H165" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="166" spans="2:9">
+      <c r="B166" t="s">
+        <v>605</v>
+      </c>
+      <c r="F166" t="s">
+        <v>20</v>
+      </c>
+      <c r="H166" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="167" spans="2:9">
+      <c r="B167" t="s">
+        <v>607</v>
+      </c>
+      <c r="F167" t="s">
+        <v>20</v>
+      </c>
+      <c r="H167" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="168" spans="2:9">
+      <c r="B168" t="s">
+        <v>608</v>
+      </c>
+      <c r="H168" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="169" spans="2:9">
+      <c r="B169" t="s">
+        <v>609</v>
+      </c>
+      <c r="H169" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="170" spans="2:9">
+      <c r="B170" t="s">
+        <v>610</v>
+      </c>
+      <c r="H170" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="171" spans="2:9">
+      <c r="B171" t="s">
+        <v>611</v>
+      </c>
+      <c r="H171" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="172" spans="2:9">
+      <c r="B172" t="s">
+        <v>613</v>
+      </c>
+      <c r="H172" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="173" spans="2:9">
+      <c r="B173" t="s">
+        <v>614</v>
+      </c>
+      <c r="H173" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="174" spans="2:9">
+      <c r="B174" t="s">
+        <v>615</v>
+      </c>
+      <c r="H174" t="s">
+        <v>572</v>
+      </c>
+      <c r="I174" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="175" spans="2:9">
+      <c r="B175" t="s">
+        <v>617</v>
+      </c>
+      <c r="H175" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="176" spans="2:9">
+      <c r="B176" t="s">
+        <v>619</v>
+      </c>
+      <c r="H176" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="177" spans="2:10">
+      <c r="B177" t="s">
+        <v>620</v>
+      </c>
+      <c r="H177" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="178" spans="2:10">
+      <c r="B178" t="s">
+        <v>621</v>
+      </c>
+      <c r="H178" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="166" spans="2:10">
-      <c r="B166" t="s">
-        <v>596</v>
-      </c>
-      <c r="H166" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="167" spans="2:10">
-      <c r="B167" t="s">
-        <v>597</v>
-      </c>
-      <c r="H167" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="168" spans="2:10">
-      <c r="B168" t="s">
-        <v>598</v>
-      </c>
-      <c r="H168" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="169" spans="2:10">
-      <c r="B169" t="s">
-        <v>600</v>
-      </c>
-      <c r="H169" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="170" spans="2:10">
-      <c r="B170" t="s">
-        <v>601</v>
-      </c>
-      <c r="H170" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="171" spans="2:10">
-      <c r="B171" t="s">
-        <v>602</v>
-      </c>
-      <c r="H171" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="172" spans="2:10">
-      <c r="B172" t="s">
-        <v>603</v>
-      </c>
-      <c r="H172" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="173" spans="2:10">
-      <c r="B173" t="s">
-        <v>605</v>
-      </c>
-      <c r="H173" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="174" spans="2:10">
-      <c r="B174" t="s">
-        <v>606</v>
-      </c>
-      <c r="H174" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="175" spans="2:10">
-      <c r="B175" t="s">
-        <v>607</v>
-      </c>
-      <c r="H175" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="176" spans="2:10">
-      <c r="B176" t="s">
-        <v>608</v>
-      </c>
-      <c r="F176" t="s">
-        <v>20</v>
-      </c>
-      <c r="H176" t="s">
-        <v>76</v>
-      </c>
-      <c r="J176" t="s">
-        <v>609</v>
+    <row r="179" spans="2:10">
+      <c r="B179" t="s">
+        <v>622</v>
+      </c>
+      <c r="F179" t="s">
+        <v>20</v>
+      </c>
+      <c r="H179" t="s">
+        <v>81</v>
+      </c>
+      <c r="J179" t="s">
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -5318,44 +5426,44 @@
     <hyperlink ref="B34" r:id="rId33"/>
     <hyperlink ref="B35" r:id="rId34"/>
     <hyperlink ref="B36" r:id="rId35"/>
-    <hyperlink ref="B38" r:id="rId36"/>
-    <hyperlink ref="B39" r:id="rId37"/>
-    <hyperlink ref="B40" r:id="rId38"/>
+    <hyperlink ref="B37" r:id="rId36"/>
+    <hyperlink ref="B38" r:id="rId37"/>
+    <hyperlink ref="B39" r:id="rId38"/>
     <hyperlink ref="B41" r:id="rId39"/>
     <hyperlink ref="B42" r:id="rId40"/>
     <hyperlink ref="B43" r:id="rId41"/>
-    <hyperlink ref="B45" r:id="rId42"/>
-    <hyperlink ref="B46" r:id="rId43"/>
-    <hyperlink ref="B47" r:id="rId44"/>
+    <hyperlink ref="B44" r:id="rId42"/>
+    <hyperlink ref="B45" r:id="rId43"/>
+    <hyperlink ref="B46" r:id="rId44"/>
     <hyperlink ref="B48" r:id="rId45"/>
     <hyperlink ref="B49" r:id="rId46"/>
-    <hyperlink ref="B53" r:id="rId47"/>
-    <hyperlink ref="B55" r:id="rId48"/>
-    <hyperlink ref="B56" r:id="rId49"/>
-    <hyperlink ref="B57" r:id="rId50"/>
+    <hyperlink ref="B50" r:id="rId47"/>
+    <hyperlink ref="B51" r:id="rId48"/>
+    <hyperlink ref="B52" r:id="rId49"/>
+    <hyperlink ref="B56" r:id="rId50"/>
     <hyperlink ref="B58" r:id="rId51"/>
     <hyperlink ref="B59" r:id="rId52"/>
     <hyperlink ref="B60" r:id="rId53"/>
     <hyperlink ref="B61" r:id="rId54"/>
-    <hyperlink ref="B63" r:id="rId55"/>
-    <hyperlink ref="B64" r:id="rId56"/>
-    <hyperlink ref="B65" r:id="rId57"/>
+    <hyperlink ref="B62" r:id="rId55"/>
+    <hyperlink ref="B63" r:id="rId56"/>
+    <hyperlink ref="B64" r:id="rId57"/>
     <hyperlink ref="B66" r:id="rId58"/>
     <hyperlink ref="B67" r:id="rId59"/>
     <hyperlink ref="B68" r:id="rId60"/>
-    <hyperlink ref="B70" r:id="rId61"/>
-    <hyperlink ref="B71" r:id="rId62"/>
-    <hyperlink ref="B72" r:id="rId63"/>
+    <hyperlink ref="B69" r:id="rId61"/>
+    <hyperlink ref="B70" r:id="rId62"/>
+    <hyperlink ref="B71" r:id="rId63"/>
     <hyperlink ref="B73" r:id="rId64"/>
     <hyperlink ref="B74" r:id="rId65"/>
     <hyperlink ref="B75" r:id="rId66"/>
     <hyperlink ref="B76" r:id="rId67"/>
     <hyperlink ref="B77" r:id="rId68"/>
     <hyperlink ref="B78" r:id="rId69"/>
-    <hyperlink ref="B80" r:id="rId70"/>
-    <hyperlink ref="B82" r:id="rId71"/>
-    <hyperlink ref="B83" r:id="rId72"/>
-    <hyperlink ref="B84" r:id="rId73"/>
+    <hyperlink ref="B79" r:id="rId70"/>
+    <hyperlink ref="B80" r:id="rId71"/>
+    <hyperlink ref="B81" r:id="rId72"/>
+    <hyperlink ref="B83" r:id="rId73"/>
     <hyperlink ref="B85" r:id="rId74"/>
     <hyperlink ref="B86" r:id="rId75"/>
     <hyperlink ref="B87" r:id="rId76"/>
@@ -5386,17 +5494,17 @@
     <hyperlink ref="B112" r:id="rId101"/>
     <hyperlink ref="B113" r:id="rId102"/>
     <hyperlink ref="B114" r:id="rId103"/>
-    <hyperlink ref="B116" r:id="rId104"/>
-    <hyperlink ref="B117" r:id="rId105"/>
-    <hyperlink ref="B118" r:id="rId106"/>
+    <hyperlink ref="B115" r:id="rId104"/>
+    <hyperlink ref="B116" r:id="rId105"/>
+    <hyperlink ref="B117" r:id="rId106"/>
     <hyperlink ref="B119" r:id="rId107"/>
     <hyperlink ref="B120" r:id="rId108"/>
     <hyperlink ref="B121" r:id="rId109"/>
     <hyperlink ref="B122" r:id="rId110"/>
     <hyperlink ref="B123" r:id="rId111"/>
-    <hyperlink ref="B125" r:id="rId112"/>
-    <hyperlink ref="B126" r:id="rId113"/>
-    <hyperlink ref="B127" r:id="rId114"/>
+    <hyperlink ref="B124" r:id="rId112"/>
+    <hyperlink ref="B125" r:id="rId113"/>
+    <hyperlink ref="B126" r:id="rId114"/>
     <hyperlink ref="B128" r:id="rId115"/>
     <hyperlink ref="B129" r:id="rId116"/>
     <hyperlink ref="B130" r:id="rId117"/>
@@ -5446,6 +5554,9 @@
     <hyperlink ref="B174" r:id="rId161"/>
     <hyperlink ref="B175" r:id="rId162"/>
     <hyperlink ref="B176" r:id="rId163"/>
+    <hyperlink ref="B177" r:id="rId164"/>
+    <hyperlink ref="B178" r:id="rId165"/>
+    <hyperlink ref="B179" r:id="rId166"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>